<commit_message>
added async operations with db
</commit_message>
<xml_diff>
--- a/ResultsOfTheSessionNUnitTest/PreparationOfReportsNUnitTest/Resources/SessionResultForGroup.xlsx
+++ b/ResultsOfTheSessionNUnitTest/PreparationOfReportsNUnitTest/Resources/SessionResultForGroup.xlsx
@@ -202,13 +202,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,228 +243,228 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" ht="20" customHeight="1" s="1" customFormat="1">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" ht="20" customHeight="1" s="1" customFormat="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -504,228 +501,228 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" ht="20" customHeight="1" s="1" customFormat="1">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" ht="20" customHeight="1" s="1" customFormat="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>